<commit_message>
问题描述：screen size data list
解决方法：
</commit_message>
<xml_diff>
--- a/test/screen_size.xlsx
+++ b/test/screen_size.xlsx
@@ -415,7 +415,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>

</xml_diff>